<commit_message>
updating of notebooks for validation and test split
</commit_message>
<xml_diff>
--- a/Data/Variable_Explanation.xlsx
+++ b/Data/Variable_Explanation.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lucal\Documents\HSG\7._Semester\Business_Analytics_&amp;_Data_Science_Applications\Capstone\Business-Analytics\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lucal\Documents\HSG\7._Semester\Business_Analytics_&amp;_Data_Science_Applications\Capstone\Business-Analytics\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{1754EE91-7EB9-4C37-BC4E-BAF384CD99A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6E38EB2-CBDC-44FD-B939-0CF1EF51348D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{05264093-7164-4A32-B4EE-B71DB2870517}"/>
   </bookViews>
@@ -132,9 +132,6 @@
     <t>Revenue</t>
   </si>
   <si>
-    <t>Klassenbezeichnung, die angibt, ob der Besuch mit einer Transaktion abgeschlossen wurde. 1 bedeutet Transaktion und 0 bedeutet keine Transaktion</t>
-  </si>
-  <si>
     <t>Gesamtzeit (in Sekunden), die ein Besucher auf den Informationsseiten verbracht hat</t>
   </si>
   <si>
@@ -148,6 +145,9 @@
   </si>
   <si>
     <t>Durchschnittlicher Wert in US-Dollar der besuchten Seiten basierend auf Google Analytics</t>
+  </si>
+  <si>
+    <t>Zielvariable: (0)/1 bedeutet (keine)/Transaktion am Ende eines Website Besuchs</t>
   </si>
 </sst>
 </file>
@@ -578,8 +578,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{74192A45-E16D-4B8A-A3E0-2640396E9FB1}">
   <dimension ref="A1:B19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:B19"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -612,7 +612,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="91.8" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="3" t="s">
         <v>6</v>
       </c>
@@ -625,15 +625,15 @@
         <v>8</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" ht="57.6" thickBot="1" x14ac:dyDescent="0.35">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" s="3" t="s">
         <v>9</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="69" thickBot="1" x14ac:dyDescent="0.35">
@@ -641,10 +641,10 @@
         <v>10</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" ht="69" thickBot="1" x14ac:dyDescent="0.35">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A8" s="3" t="s">
         <v>11</v>
       </c>
@@ -652,23 +652,23 @@
         <v>12</v>
       </c>
     </row>
-    <row r="9" spans="1:2" ht="69" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A9" s="3" t="s">
         <v>13</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" ht="80.400000000000006" thickBot="1" x14ac:dyDescent="0.35">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A10" s="3" t="s">
         <v>14</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" ht="57.6" thickBot="1" x14ac:dyDescent="0.35">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="3" t="s">
         <v>15</v>
       </c>
@@ -676,7 +676,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="12" spans="1:2" ht="23.4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12" s="3" t="s">
         <v>17</v>
       </c>
@@ -684,7 +684,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="13" spans="1:2" ht="23.4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A13" s="3" t="s">
         <v>19</v>
       </c>
@@ -692,7 +692,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="14" spans="1:2" ht="23.4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A14" s="3" t="s">
         <v>21</v>
       </c>
@@ -700,7 +700,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="15" spans="1:2" ht="57.6" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A15" s="3" t="s">
         <v>23</v>
       </c>
@@ -708,7 +708,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="16" spans="1:2" ht="69" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A16" s="3" t="s">
         <v>25</v>
       </c>
@@ -716,7 +716,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="17" spans="1:2" ht="69" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A17" s="3" t="s">
         <v>27</v>
       </c>
@@ -724,7 +724,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="18" spans="1:2" ht="69" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A18" s="3" t="s">
         <v>29</v>
       </c>
@@ -732,12 +732,12 @@
         <v>30</v>
       </c>
     </row>
-    <row r="19" spans="1:2" ht="126" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A19" s="3" t="s">
         <v>31</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
     </row>
   </sheetData>

</xml_diff>